<commit_message>
draft attempt at getting dialougs
key approuch didn't pan out - commiting to get back to it just incase -
will try getting the dilougs directly instead
</commit_message>
<xml_diff>
--- a/src/assets/AwkwardAnnieDialogContent_all.xlsx
+++ b/src/assets/AwkwardAnnieDialogContent_all.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26400" windowHeight="15940" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="9960" yWindow="1140" windowWidth="26400" windowHeight="15940" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="templateFullPostive" sheetId="1" r:id="rId1"/>
@@ -7864,8 +7864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28680,8 +28680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -28926,9 +28926,7 @@
       <c r="B12" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>45</v>
-      </c>
+      <c r="C12" s="22"/>
       <c r="D12" s="23" t="s">
         <v>12</v>
       </c>
@@ -28941,7 +28939,9 @@
       <c r="B13" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="22"/>
+      <c r="C13" s="24" t="s">
+        <v>46</v>
+      </c>
       <c r="D13" s="23" t="s">
         <v>19</v>
       </c>
@@ -29353,7 +29353,7 @@
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="K1:L1"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D11:D15 D17:D21 D23:D27 D29:D33 D35:D38 D40:D43">
       <formula1>$I$3:$I$7</formula1>
       <formula2>0</formula2>
@@ -40347,7 +40347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
@@ -41626,7 +41626,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG1048576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E2" workbookViewId="0">
+    <sheetView topLeftCell="E2" workbookViewId="0">
       <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>

</xml_diff>